<commit_message>
Refactor sync architecture to use server-side processing
- Create shared Google Sheets utilities module (lib/google-sheets.js)
- Refactor all content sync endpoints to fetch data server-side
- Simplify Google Apps Script (remove all parsing logic)
- Centralize data parsing and validation in Next.js
- Update documentation with new architecture

Benefits:
- Consistent sync patterns across all endpoints
- Easier maintenance and testing
- Better error handling and logging
- Simplified Apps Script (~55% code reduction)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/content-data-template.xlsx
+++ b/content-data-template.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -536,6 +536,74 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>cuid_fin_202403</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2024-03-01</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>125000.5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>97250.75</v>
+      </c>
+      <c r="E4" t="n">
+        <v>27749.75</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Mar 2024 Ministry Update</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>[{"id":"tithes","label":"ถวายสิบลด","amount":82000},{"id":"partnerships","label":"Partnership Gifts","amount":43000}]</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>[{"id":"operations","label":"ค่าใช้จ่ายดำเนินงาน","amount":32000},{"id":"missions","label":"Missions Support","amount":22000},{"id":"staff","label":"Staff Salaries","amount":43250.75}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>118500</v>
+      </c>
+      <c r="D5" t="n">
+        <v>110200</v>
+      </c>
+      <c r="E5" t="n">
+        <v>20049.75</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Apr 2024 Easter Activities</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>[{"id":"donations","label":"Easter Offering","amount":45500},{"id":"grants","label":"Community Grant","amount":73000}]</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>[{"id":"outreach","label":"Outreach Events","amount":42000},{"id":"benevolence","label":"Benevolence","amount":18500},{"id":"facilities","label":"Facility Upgrades","amount":49600}]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
@@ -550,7 +618,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -649,6 +717,60 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>cuid_proj_center</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Community Center Renovation</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Upgrade the main hall and classrooms to expand youth programs.</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>500000</v>
+      </c>
+      <c r="E4" t="n">
+        <v>185000</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Mobile Medical Clinic</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Equip a mobile team to provide basic care in rural villages.</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>350000</v>
+      </c>
+      <c r="E5" t="n">
+        <v>45000</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
@@ -663,7 +785,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -927,6 +1049,116 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>cuid_mission_youth</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>chiang-mai-youth</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>พันธกิจเยาวชนเชียงใหม่</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Chiang Mai Youth Outreach</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>สร้างผู้นำรุ่นใหม่</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Raising Young Leaders</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>ทำงานร่วมกับคริสตจักรท้องถิ่นเพื่อเสริมสร้างเยาวชนให้เติบโตเป็นสาวก</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Partner with local churches to equip students as disciples.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>ทีมงานจัดค่าย การอบรม และการติดตามผลเพื่อสนับสนุนเยาวชนและครอบครัวตลอดปี</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>The team runs camps, leadership labs, and follow-up coaching with families year-round.</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>ค่ายเยาวชน | การเป็นผู้นำ | ศิลปะสร้างสรรค์</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Youth Camps | Leadership Labs | Creative Arts</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>มัทธิว 5:14</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Matthew 5:14</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>ท่านทั้งหลายเป็นความสว่างของโลก...</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>You are the light of the world...</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>อธิษฐานสนับสนุน | ร่วมอาสา | ให้การสนับสนุนทางการเงิน</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Pray with us | Volunteer on-site | Become a monthly partner</t>
+        </is>
+      </c>
+      <c r="S4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>https://example.org/images/chiang-mai-youth.jpg</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>2024-12-15</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:V1"/>
@@ -941,7 +1173,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -1117,6 +1349,74 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>คริสตจักรความหวังกรุงเทพ</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Hope Church Bangkok</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>02-123-4567, 081-234-5678</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>office@hopebkk.org</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>123 ถนนสุขุมวิท แขวงคลองตัน เขตคลองเตย กรุงเทพฯ 10110</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>123 Sukhumvit Rd, Khlong Toei, Bangkok 10110</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>https://facebook.com/hopechurchbkk</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>https://facebook.com/hopechurchbkk/live</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>https://youtube.com/@hopechurchbkk</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>https://maps.google.com/?q=13.73,100.567</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>13.73</v>
+      </c>
+      <c r="M4" t="n">
+        <v>100.567</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Sunday|09:30|Thai Service
+Sunday|11:30|English Service
+Wednesday|19:00|Prayer Gathering</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:N1"/>
@@ -1131,7 +1431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -1219,6 +1519,86 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>cuid_nav_home</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>หน้าแรก</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>cuid_nav_missions</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>พันธกิจ</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Missions</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>/missions</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ถวาย</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Give</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>/give</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
@@ -1233,7 +1613,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -1376,6 +1756,116 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>cuid_page_landing_hero</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>landing</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>hero</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ยินดีต้อนรับสู่คริสตจักร</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Welcome to Our Church</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>ครอบครัวที่เติบโตไปด้วยกัน</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>A family growing together</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>เรามุ่งมั่นที่จะเห็นชีวิตได้รับการเปลี่ยนแปลงผ่านการติดตามพระเยซู</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>We pursue transformed lives through following Jesus together.</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>{"ctaLabel":"Join Us","ctaHref":"/contact"}</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>{"background":"sunrise","metaDescription":"Hope Church Bangkok landing hero"}</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>landing</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>stories</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>คำพยานล่าสุด</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Latest Stories</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>พระเจ้าทรงทำสิ่งใหม่</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>God is doing something new</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>สมาชิกของเรามีประสบการณ์ที่พระเจ้าทรงเปลี่ยนแปลงชีวิตทุกสัปดาห์</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Every week our members share how God is changing lives.</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>[{"name":"Nok","highlight":"Found freedom from anxiety"},{"name":"Ben","highlight":"Started discipling teens"}]</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>{"showFilter":true}</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>
@@ -1390,7 +1880,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1499,7 +1989,96 @@
         </is>
       </c>
     </row>
-    <row r="4"/>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>cuid_cat_tithes</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>tithes</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Tithes &amp; Offerings</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>income</t>
+        </is>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>cuid_cat_missions</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>missions</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Missions Support</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>expense</t>
+        </is>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>administration</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Administration</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>expense</t>
+        </is>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>operations</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2024</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1565,7 +2144,21 @@
         </is>
       </c>
     </row>
-    <row r="4"/>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>cuid_settings_2024</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2024</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>{"featuredCategories":["tithes","missions"],"monthlyGoal":450000,"showCumulative":true}</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>